<commit_message>
update on lexeme code
</commit_message>
<xml_diff>
--- a/FSM Table.xlsx
+++ b/FSM Table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\97ran\Desktop\Lexical-Analyzer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\97randy\Desktop\Lexical-Analyzer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1EE249-F408-4749-B05F-8FB1EC2B58BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AAD0F7D-72E6-4A54-BA0C-9EA698DE23CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10040" xr2:uid="{64FDED9E-DD93-470E-A362-5A4DBBF53418}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="10035" xr2:uid="{64FDED9E-DD93-470E-A362-5A4DBBF53418}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -465,15 +465,15 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="38.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="38.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -500,7 +500,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -529,7 +529,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -558,7 +558,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -587,7 +587,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -616,7 +616,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -645,7 +645,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -674,7 +674,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -703,7 +703,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -732,7 +732,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -761,7 +761,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>

</xml_diff>